<commit_message>
Chest, Mimic, fix Piston
</commit_message>
<xml_diff>
--- a/bug finder.xlsx
+++ b/bug finder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Tech demo platformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315866C1-B94C-4E35-9298-8E9D92ED5E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D358D445-4C92-4DB8-A94D-0FE6820AC894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="21000" xr2:uid="{9356C0CF-D086-4FEC-A8F0-753CF5CB4E4B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="114">
   <si>
     <t>A</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>lỗi gravity</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Mimic</t>
   </si>
 </sst>
 </file>
@@ -451,7 +457,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -551,6 +557,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -834,6 +846,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,13 +1167,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:AZ59"/>
+  <dimension ref="A1:BB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S55" sqref="S55"/>
+      <selection pane="bottomRight" activeCell="AC83" sqref="AC83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.35"/>
@@ -1187,25 +1202,26 @@
     <col min="30" max="30" width="15.5703125" style="22" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14.28515625" style="22" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="19.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.140625" style="22" customWidth="1"/>
     <col min="34" max="34" width="12.85546875" style="22" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="20.85546875" style="22" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="9" style="22" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="18.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="18.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="24.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="35.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="50" max="52" width="9" style="22" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="22"/>
+    <col min="38" max="38" width="9" style="22" customWidth="1"/>
+    <col min="39" max="39" width="18.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="24.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="35.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="51" max="53" width="9" style="22" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="50"/>
       <c r="B1" s="51"/>
       <c r="C1" s="3" t="s">
@@ -1240,14 +1256,14 @@
       </c>
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="5"/>
+      <c r="AD1" s="7"/>
       <c r="AE1" s="5"/>
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
@@ -1262,20 +1278,22 @@
       <c r="AP1" s="5"/>
       <c r="AQ1" s="5"/>
       <c r="AR1" s="5"/>
-      <c r="AS1" s="8" t="s">
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
       <c r="AV1" s="8"/>
-      <c r="AW1" s="9" t="s">
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="AX1" s="9"/>
-      <c r="AY1" s="9"/>
       <c r="AZ1" s="9"/>
-    </row>
-    <row r="2" spans="1:52" s="15" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="BA1" s="9"/>
+      <c r="BB1" s="9"/>
+    </row>
+    <row r="2" spans="1:54" s="15" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="52"/>
       <c r="B2" s="53"/>
       <c r="C2" s="11" t="s">
@@ -1348,88 +1366,94 @@
         <v>29</v>
       </c>
       <c r="Z2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AB2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AB2" s="15" t="s">
+      <c r="AC2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AD2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AD2" s="11" t="s">
+      <c r="AE2" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AF2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AF2" s="11" t="s">
+      <c r="AG2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="11" t="s">
+      <c r="AH2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AH2" s="11" t="s">
+      <c r="AI2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AI2" s="11" t="s">
+      <c r="AJ2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="AJ2" s="11" t="s">
+      <c r="AK2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AK2" s="11" t="s">
+      <c r="AL2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="AL2" s="11" t="s">
+      <c r="AM2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="AN2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AM2" s="11" t="s">
+      <c r="AO2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AN2" s="11" t="s">
+      <c r="AP2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" s="11" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="AP2" s="11" t="s">
+      <c r="AR2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="AQ2" s="11" t="s">
+      <c r="AS2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AR2" s="11" t="s">
+      <c r="AT2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AS2" s="16" t="s">
+      <c r="AU2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AT2" s="16" t="s">
+      <c r="AV2" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AU2" s="16" t="s">
+      <c r="AW2" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="AV2" s="16" t="s">
+      <c r="AX2" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="AW2" s="17" t="s">
+      <c r="AY2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AX2" s="17" t="s">
+      <c r="AZ2" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="AY2" s="17" t="s">
+      <c r="BA2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AZ2" s="17" t="s">
+      <c r="BB2" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>14</v>
       </c>
@@ -1486,8 +1510,10 @@
       <c r="AX3" s="21"/>
       <c r="AY3" s="21"/>
       <c r="AZ3" s="21"/>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA3" s="21"/>
+      <c r="BB3" s="21"/>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
         <v>8</v>
@@ -1542,8 +1568,10 @@
       <c r="AX4" s="21"/>
       <c r="AY4" s="21"/>
       <c r="AZ4" s="21"/>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA4" s="21"/>
+      <c r="BB4" s="21"/>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
         <v>9</v>
@@ -1598,8 +1626,10 @@
       <c r="AX5" s="21"/>
       <c r="AY5" s="21"/>
       <c r="AZ5" s="21"/>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA5" s="21"/>
+      <c r="BB5" s="21"/>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
         <v>10</v>
@@ -1654,8 +1684,10 @@
       <c r="AX6" s="21"/>
       <c r="AY6" s="21"/>
       <c r="AZ6" s="21"/>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA6" s="21"/>
+      <c r="BB6" s="21"/>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
         <v>74</v>
@@ -1710,8 +1742,10 @@
       <c r="AX7" s="21"/>
       <c r="AY7" s="21"/>
       <c r="AZ7" s="21"/>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA7" s="21"/>
+      <c r="BB7" s="21"/>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
         <v>11</v>
@@ -1766,8 +1800,10 @@
       <c r="AX8" s="21"/>
       <c r="AY8" s="21"/>
       <c r="AZ8" s="21"/>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA8" s="21"/>
+      <c r="BB8" s="21"/>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A9" s="18"/>
       <c r="B9" s="19" t="s">
         <v>12</v>
@@ -1822,8 +1858,10 @@
       <c r="AX9" s="21"/>
       <c r="AY9" s="21"/>
       <c r="AZ9" s="21"/>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA9" s="21"/>
+      <c r="BB9" s="21"/>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A10" s="18"/>
       <c r="B10" s="19" t="s">
         <v>39</v>
@@ -1880,8 +1918,10 @@
       <c r="AX10" s="21"/>
       <c r="AY10" s="21"/>
       <c r="AZ10" s="21"/>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA10" s="21"/>
+      <c r="BB10" s="21"/>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="s">
         <v>13</v>
@@ -1936,8 +1976,10 @@
       <c r="AX11" s="21"/>
       <c r="AY11" s="21"/>
       <c r="AZ11" s="21"/>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA11" s="21"/>
+      <c r="BB11" s="21"/>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>21</v>
       </c>
@@ -1996,8 +2038,10 @@
       <c r="AX12" s="21"/>
       <c r="AY12" s="21"/>
       <c r="AZ12" s="21"/>
-    </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA12" s="21"/>
+      <c r="BB12" s="21"/>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A13" s="26"/>
       <c r="B13" s="27" t="s">
         <v>16</v>
@@ -2056,8 +2100,10 @@
       <c r="AX13" s="21"/>
       <c r="AY13" s="21"/>
       <c r="AZ13" s="21"/>
-    </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA13" s="21"/>
+      <c r="BB13" s="21"/>
+    </row>
+    <row r="14" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A14" s="26"/>
       <c r="B14" s="27" t="s">
         <v>17</v>
@@ -2114,8 +2160,10 @@
       <c r="AX14" s="21"/>
       <c r="AY14" s="21"/>
       <c r="AZ14" s="21"/>
-    </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA14" s="21"/>
+      <c r="BB14" s="21"/>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A15" s="26"/>
       <c r="B15" s="27" t="s">
         <v>33</v>
@@ -2174,8 +2222,10 @@
       <c r="AX15" s="21"/>
       <c r="AY15" s="21"/>
       <c r="AZ15" s="21"/>
-    </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA15" s="21"/>
+      <c r="BB15" s="21"/>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A16" s="26"/>
       <c r="B16" s="27" t="s">
         <v>18</v>
@@ -2232,8 +2282,10 @@
       <c r="AX16" s="21"/>
       <c r="AY16" s="21"/>
       <c r="AZ16" s="21"/>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA16" s="21"/>
+      <c r="BB16" s="21"/>
+    </row>
+    <row r="17" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A17" s="26"/>
       <c r="B17" s="27" t="s">
         <v>19</v>
@@ -2290,8 +2342,10 @@
       <c r="AX17" s="21"/>
       <c r="AY17" s="21"/>
       <c r="AZ17" s="21"/>
-    </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA17" s="21"/>
+      <c r="BB17" s="21"/>
+    </row>
+    <row r="18" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>
       <c r="B18" s="27" t="s">
         <v>20</v>
@@ -2348,8 +2402,10 @@
       <c r="AX18" s="21"/>
       <c r="AY18" s="21"/>
       <c r="AZ18" s="21"/>
-    </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA18" s="21"/>
+      <c r="BB18" s="21"/>
+    </row>
+    <row r="19" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A19" s="29" t="s">
         <v>26</v>
       </c>
@@ -2414,8 +2470,10 @@
       <c r="AX19" s="21"/>
       <c r="AY19" s="21"/>
       <c r="AZ19" s="21"/>
-    </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA19" s="21"/>
+      <c r="BB19" s="21"/>
+    </row>
+    <row r="20" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A20" s="29"/>
       <c r="B20" s="30" t="s">
         <v>22</v>
@@ -2482,8 +2540,10 @@
       <c r="AX20" s="21"/>
       <c r="AY20" s="21"/>
       <c r="AZ20" s="21"/>
-    </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA20" s="21"/>
+      <c r="BB20" s="21"/>
+    </row>
+    <row r="21" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A21" s="29"/>
       <c r="B21" s="30" t="s">
         <v>23</v>
@@ -2538,8 +2598,10 @@
       <c r="AX21" s="21"/>
       <c r="AY21" s="21"/>
       <c r="AZ21" s="21"/>
-    </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA21" s="21"/>
+      <c r="BB21" s="21"/>
+    </row>
+    <row r="22" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A22" s="29"/>
       <c r="B22" s="30" t="s">
         <v>24</v>
@@ -2594,8 +2656,10 @@
       <c r="AX22" s="21"/>
       <c r="AY22" s="21"/>
       <c r="AZ22" s="21"/>
-    </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA22" s="21"/>
+      <c r="BB22" s="21"/>
+    </row>
+    <row r="23" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A23" s="29"/>
       <c r="B23" s="30" t="s">
         <v>25</v>
@@ -2654,8 +2718,10 @@
       <c r="AX23" s="21"/>
       <c r="AY23" s="21"/>
       <c r="AZ23" s="21"/>
-    </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA23" s="21"/>
+      <c r="BB23" s="21"/>
+    </row>
+    <row r="24" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A24" s="31" t="s">
         <v>27</v>
       </c>
@@ -2730,8 +2796,10 @@
       <c r="AX24" s="21"/>
       <c r="AY24" s="21"/>
       <c r="AZ24" s="21"/>
-    </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA24" s="21"/>
+      <c r="BB24" s="21"/>
+    </row>
+    <row r="25" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A25" s="31"/>
       <c r="B25" s="32" t="s">
         <v>29</v>
@@ -2814,41 +2882,37 @@
       <c r="AX25" s="21"/>
       <c r="AY25" s="21"/>
       <c r="AZ25" s="21"/>
-    </row>
-    <row r="26" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA25" s="21"/>
+      <c r="BB25" s="21"/>
+    </row>
+    <row r="26" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A26" s="31"/>
       <c r="B26" s="32" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="24" t="s">
-        <v>66</v>
-      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="20"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
       <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="24" t="s">
-        <v>101</v>
-      </c>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
       <c r="T26" s="20"/>
       <c r="U26" s="20"/>
       <c r="V26" s="20"/>
-      <c r="W26" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20"/>
       <c r="Z26" s="20"/>
       <c r="AA26" s="21"/>
       <c r="AB26" s="21"/>
@@ -2876,31 +2940,25 @@
       <c r="AX26" s="21"/>
       <c r="AY26" s="21"/>
       <c r="AZ26" s="21"/>
-    </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A27" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>31</v>
+      <c r="BA26" s="21"/>
+      <c r="BB26" s="21"/>
+    </row>
+    <row r="27" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A27" s="31"/>
+      <c r="B27" s="32" t="s">
+        <v>48</v>
       </c>
       <c r="C27" s="20"/>
-      <c r="D27" s="24"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="I27" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="J27" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="K27" s="24" t="s">
-        <v>87</v>
-      </c>
+      <c r="F27" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
       <c r="L27" s="20"/>
       <c r="M27" s="20"/>
       <c r="N27" s="20"/>
@@ -2908,16 +2966,18 @@
       <c r="P27" s="20"/>
       <c r="Q27" s="20"/>
       <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="24" t="s">
-        <v>78</v>
-      </c>
+      <c r="S27" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="T27" s="20"/>
       <c r="U27" s="20"/>
       <c r="V27" s="20"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="20"/>
-      <c r="Y27" s="20"/>
-      <c r="Z27" s="20"/>
+      <c r="W27" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="X27" s="24"/>
+      <c r="Y27" s="24"/>
+      <c r="Z27" s="24"/>
       <c r="AA27" s="20"/>
       <c r="AB27" s="21"/>
       <c r="AC27" s="21"/>
@@ -2944,36 +3004,47 @@
       <c r="AX27" s="21"/>
       <c r="AY27" s="21"/>
       <c r="AZ27" s="21"/>
-    </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A28" s="29" t="s">
-        <v>32</v>
+      <c r="BA27" s="21"/>
+      <c r="BB27" s="21"/>
+    </row>
+    <row r="28" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A28" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>63</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C28" s="20"/>
       <c r="D28" s="24"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="K28" s="24" t="s">
+        <v>87</v>
+      </c>
       <c r="L28" s="20"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
       <c r="P28" s="20"/>
       <c r="Q28" s="20"/>
       <c r="R28" s="20"/>
       <c r="S28" s="20"/>
-      <c r="T28" s="20"/>
+      <c r="T28" s="24" t="s">
+        <v>78</v>
+      </c>
       <c r="U28" s="20"/>
       <c r="V28" s="20"/>
-      <c r="W28" s="20"/>
+      <c r="W28" s="24"/>
       <c r="X28" s="20"/>
       <c r="Y28" s="20"/>
       <c r="Z28" s="20"/>
@@ -3003,17 +3074,22 @@
       <c r="AX28" s="21"/>
       <c r="AY28" s="21"/>
       <c r="AZ28" s="21"/>
-    </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A29" s="29"/>
+      <c r="BA28" s="21"/>
+      <c r="BB28" s="21"/>
+    </row>
+    <row r="29" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A29" s="29" t="s">
+        <v>32</v>
+      </c>
       <c r="B29" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="20"/>
+        <v>63</v>
+      </c>
       <c r="D29" s="24"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="44"/>
+      <c r="G29" s="24" t="s">
+        <v>75</v>
+      </c>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20"/>
@@ -3059,17 +3135,19 @@
       <c r="AX29" s="21"/>
       <c r="AY29" s="21"/>
       <c r="AZ29" s="21"/>
-    </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA29" s="21"/>
+      <c r="BB29" s="21"/>
+    </row>
+    <row r="30" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A30" s="29"/>
       <c r="B30" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="24"/>
+        <v>62</v>
+      </c>
+      <c r="C30" s="20"/>
       <c r="D30" s="24"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
+      <c r="G30" s="44"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="20"/>
@@ -3115,11 +3193,13 @@
       <c r="AX30" s="21"/>
       <c r="AY30" s="21"/>
       <c r="AZ30" s="21"/>
-    </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA30" s="21"/>
+      <c r="BB30" s="21"/>
+    </row>
+    <row r="31" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A31" s="29"/>
       <c r="B31" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
@@ -3171,17 +3251,19 @@
       <c r="AX31" s="21"/>
       <c r="AY31" s="21"/>
       <c r="AZ31" s="21"/>
-    </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA31" s="21"/>
+      <c r="BB31" s="21"/>
+    </row>
+    <row r="32" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A32" s="29"/>
       <c r="B32" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="20"/>
+        <v>59</v>
+      </c>
+      <c r="C32" s="24"/>
       <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="20"/>
-      <c r="G32" s="24"/>
+      <c r="G32" s="20"/>
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -3189,17 +3271,17 @@
       <c r="L32" s="20"/>
       <c r="M32" s="24"/>
       <c r="N32" s="24"/>
-      <c r="O32" s="20"/>
+      <c r="O32" s="24"/>
       <c r="P32" s="20"/>
       <c r="Q32" s="20"/>
       <c r="R32" s="20"/>
-      <c r="S32" s="24"/>
+      <c r="S32" s="20"/>
       <c r="T32" s="20"/>
       <c r="U32" s="20"/>
       <c r="V32" s="20"/>
       <c r="W32" s="20"/>
-      <c r="X32" s="24"/>
-      <c r="Y32" s="24"/>
+      <c r="X32" s="20"/>
+      <c r="Y32" s="20"/>
       <c r="Z32" s="20"/>
       <c r="AA32" s="20"/>
       <c r="AB32" s="20"/>
@@ -3227,11 +3309,13 @@
       <c r="AX32" s="21"/>
       <c r="AY32" s="21"/>
       <c r="AZ32" s="21"/>
-    </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA32" s="21"/>
+      <c r="BB32" s="21"/>
+    </row>
+    <row r="33" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A33" s="29"/>
       <c r="B33" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="24"/>
@@ -3240,16 +3324,16 @@
       <c r="G33" s="24"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="24"/>
+      <c r="J33" s="20"/>
       <c r="K33" s="20"/>
-      <c r="L33" s="24"/>
+      <c r="L33" s="20"/>
       <c r="M33" s="24"/>
       <c r="N33" s="24"/>
       <c r="O33" s="20"/>
       <c r="P33" s="20"/>
       <c r="Q33" s="20"/>
       <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
+      <c r="S33" s="24"/>
       <c r="T33" s="20"/>
       <c r="U33" s="20"/>
       <c r="V33" s="20"/>
@@ -3263,7 +3347,7 @@
       <c r="AD33" s="20"/>
       <c r="AE33" s="20"/>
       <c r="AF33" s="20"/>
-      <c r="AG33" s="24"/>
+      <c r="AG33" s="20"/>
       <c r="AH33" s="21"/>
       <c r="AI33" s="21"/>
       <c r="AJ33" s="21"/>
@@ -3283,35 +3367,37 @@
       <c r="AX33" s="21"/>
       <c r="AY33" s="21"/>
       <c r="AZ33" s="21"/>
-    </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA33" s="21"/>
+      <c r="BB33" s="21"/>
+    </row>
+    <row r="34" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A34" s="29"/>
       <c r="B34" s="19" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="24"/>
-      <c r="E34" s="20"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
+      <c r="G34" s="24"/>
       <c r="H34" s="20"/>
       <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
+      <c r="J34" s="24"/>
       <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
       <c r="N34" s="24"/>
       <c r="O34" s="20"/>
       <c r="P34" s="20"/>
       <c r="Q34" s="20"/>
       <c r="R34" s="20"/>
-      <c r="S34" s="24"/>
+      <c r="S34" s="20"/>
       <c r="T34" s="20"/>
       <c r="U34" s="20"/>
       <c r="V34" s="20"/>
       <c r="W34" s="20"/>
-      <c r="X34" s="20"/>
-      <c r="Y34" s="20"/>
+      <c r="X34" s="24"/>
+      <c r="Y34" s="24"/>
       <c r="Z34" s="20"/>
       <c r="AA34" s="20"/>
       <c r="AB34" s="20"/>
@@ -3320,7 +3406,7 @@
       <c r="AE34" s="20"/>
       <c r="AF34" s="20"/>
       <c r="AG34" s="20"/>
-      <c r="AH34" s="20"/>
+      <c r="AH34" s="24"/>
       <c r="AI34" s="21"/>
       <c r="AJ34" s="21"/>
       <c r="AK34" s="21"/>
@@ -3339,11 +3425,13 @@
       <c r="AX34" s="21"/>
       <c r="AY34" s="21"/>
       <c r="AZ34" s="21"/>
-    </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA34" s="21"/>
+      <c r="BB34" s="21"/>
+    </row>
+    <row r="35" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A35" s="29"/>
       <c r="B35" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C35" s="20"/>
       <c r="D35" s="24"/>
@@ -3362,7 +3450,7 @@
       <c r="Q35" s="20"/>
       <c r="R35" s="20"/>
       <c r="S35" s="24"/>
-      <c r="T35" s="24"/>
+      <c r="T35" s="20"/>
       <c r="U35" s="20"/>
       <c r="V35" s="20"/>
       <c r="W35" s="20"/>
@@ -3395,22 +3483,24 @@
       <c r="AX35" s="21"/>
       <c r="AY35" s="21"/>
       <c r="AZ35" s="21"/>
-    </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA35" s="21"/>
+      <c r="BB35" s="21"/>
+    </row>
+    <row r="36" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A36" s="29"/>
       <c r="B36" s="19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C36" s="20"/>
       <c r="D36" s="24"/>
-      <c r="E36" s="33"/>
+      <c r="E36" s="20"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="24"/>
+      <c r="G36" s="20"/>
       <c r="H36" s="20"/>
       <c r="I36" s="20"/>
       <c r="J36" s="20"/>
       <c r="K36" s="20"/>
-      <c r="L36" s="24"/>
+      <c r="L36" s="20"/>
       <c r="M36" s="20"/>
       <c r="N36" s="24"/>
       <c r="O36" s="20"/>
@@ -3418,12 +3508,12 @@
       <c r="Q36" s="20"/>
       <c r="R36" s="20"/>
       <c r="S36" s="24"/>
-      <c r="T36" s="20"/>
+      <c r="T36" s="24"/>
       <c r="U36" s="20"/>
       <c r="V36" s="20"/>
       <c r="W36" s="20"/>
-      <c r="X36" s="28"/>
-      <c r="Y36" s="28"/>
+      <c r="X36" s="20"/>
+      <c r="Y36" s="20"/>
       <c r="Z36" s="20"/>
       <c r="AA36" s="20"/>
       <c r="AB36" s="20"/>
@@ -3431,10 +3521,10 @@
       <c r="AD36" s="20"/>
       <c r="AE36" s="20"/>
       <c r="AF36" s="20"/>
-      <c r="AG36" s="24"/>
+      <c r="AG36" s="20"/>
       <c r="AH36" s="20"/>
       <c r="AI36" s="20"/>
-      <c r="AJ36" s="24"/>
+      <c r="AJ36" s="20"/>
       <c r="AK36" s="21"/>
       <c r="AL36" s="21"/>
       <c r="AM36" s="21"/>
@@ -3451,17 +3541,19 @@
       <c r="AX36" s="21"/>
       <c r="AY36" s="21"/>
       <c r="AZ36" s="21"/>
-    </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA36" s="21"/>
+      <c r="BB36" s="21"/>
+    </row>
+    <row r="37" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A37" s="29"/>
       <c r="B37" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="20"/>
       <c r="D37" s="24"/>
-      <c r="E37" s="20"/>
+      <c r="E37" s="33"/>
       <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
+      <c r="G37" s="24"/>
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
       <c r="J37" s="20"/>
@@ -3473,13 +3565,13 @@
       <c r="P37" s="20"/>
       <c r="Q37" s="20"/>
       <c r="R37" s="20"/>
-      <c r="S37" s="20"/>
+      <c r="S37" s="24"/>
       <c r="T37" s="20"/>
       <c r="U37" s="20"/>
       <c r="V37" s="20"/>
       <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
-      <c r="Y37" s="20"/>
+      <c r="X37" s="28"/>
+      <c r="Y37" s="28"/>
       <c r="Z37" s="20"/>
       <c r="AA37" s="20"/>
       <c r="AB37" s="20"/>
@@ -3488,11 +3580,11 @@
       <c r="AE37" s="20"/>
       <c r="AF37" s="20"/>
       <c r="AG37" s="20"/>
-      <c r="AH37" s="20"/>
+      <c r="AH37" s="24"/>
       <c r="AI37" s="20"/>
       <c r="AJ37" s="20"/>
-      <c r="AK37" s="20"/>
-      <c r="AL37" s="21"/>
+      <c r="AK37" s="24"/>
+      <c r="AL37" s="55"/>
       <c r="AM37" s="21"/>
       <c r="AN37" s="21"/>
       <c r="AO37" s="21"/>
@@ -3507,35 +3599,37 @@
       <c r="AX37" s="21"/>
       <c r="AY37" s="21"/>
       <c r="AZ37" s="21"/>
-    </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA37" s="21"/>
+      <c r="BB37" s="21"/>
+    </row>
+    <row r="38" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A38" s="29"/>
       <c r="B38" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="20"/>
       <c r="D38" s="24"/>
-      <c r="E38" s="33"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
-      <c r="J38" s="24"/>
+      <c r="J38" s="20"/>
       <c r="K38" s="20"/>
       <c r="L38" s="24"/>
-      <c r="M38" s="24"/>
+      <c r="M38" s="20"/>
       <c r="N38" s="24"/>
       <c r="O38" s="20"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
       <c r="R38" s="20"/>
-      <c r="S38" s="24"/>
+      <c r="S38" s="20"/>
       <c r="T38" s="20"/>
       <c r="U38" s="20"/>
       <c r="V38" s="20"/>
-      <c r="W38" s="24"/>
-      <c r="X38" s="24"/>
-      <c r="Y38" s="24"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
       <c r="Z38" s="20"/>
       <c r="AA38" s="20"/>
       <c r="AB38" s="20"/>
@@ -3549,8 +3643,8 @@
       <c r="AJ38" s="20"/>
       <c r="AK38" s="20"/>
       <c r="AL38" s="20"/>
-      <c r="AM38" s="21"/>
-      <c r="AN38" s="21"/>
+      <c r="AM38" s="55"/>
+      <c r="AN38" s="55"/>
       <c r="AO38" s="21"/>
       <c r="AP38" s="21"/>
       <c r="AQ38" s="21"/>
@@ -3563,36 +3657,38 @@
       <c r="AX38" s="21"/>
       <c r="AY38" s="21"/>
       <c r="AZ38" s="21"/>
-    </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA38" s="21"/>
+      <c r="BB38" s="21"/>
+    </row>
+    <row r="39" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A39" s="29"/>
       <c r="B39" s="19" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="C39" s="20"/>
       <c r="D39" s="24"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="24"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="20"/>
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
       <c r="J39" s="20"/>
       <c r="K39" s="20"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="24"/>
+      <c r="L39" s="20"/>
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
       <c r="Q39" s="20"/>
       <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
+      <c r="S39" s="24"/>
       <c r="T39" s="20"/>
       <c r="U39" s="20"/>
       <c r="V39" s="20"/>
       <c r="W39" s="20"/>
-      <c r="X39" s="24"/>
-      <c r="Y39" s="24"/>
-      <c r="Z39" s="20"/>
+      <c r="X39" s="20"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="24"/>
       <c r="AA39" s="20"/>
       <c r="AB39" s="20"/>
       <c r="AC39" s="20"/>
@@ -3601,14 +3697,12 @@
       <c r="AF39" s="20"/>
       <c r="AG39" s="20"/>
       <c r="AH39" s="20"/>
-      <c r="AI39" s="20"/>
+      <c r="AI39" s="24"/>
       <c r="AJ39" s="24"/>
       <c r="AK39" s="20"/>
       <c r="AL39" s="20"/>
-      <c r="AM39" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="AN39" s="21"/>
+      <c r="AM39" s="20"/>
+      <c r="AN39" s="55"/>
       <c r="AO39" s="21"/>
       <c r="AP39" s="21"/>
       <c r="AQ39" s="21"/>
@@ -3621,20 +3715,22 @@
       <c r="AX39" s="21"/>
       <c r="AY39" s="21"/>
       <c r="AZ39" s="21"/>
-    </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA39" s="21"/>
+      <c r="BB39" s="21"/>
+    </row>
+    <row r="40" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A40" s="29"/>
       <c r="B40" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="24"/>
-      <c r="E40" s="20"/>
+      <c r="E40" s="33"/>
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
+      <c r="J40" s="24"/>
       <c r="K40" s="20"/>
       <c r="L40" s="24"/>
       <c r="M40" s="24"/>
@@ -3642,10 +3738,8 @@
       <c r="O40" s="20"/>
       <c r="P40" s="24"/>
       <c r="Q40" s="24"/>
-      <c r="R40" s="24"/>
-      <c r="S40" s="24" t="s">
-        <v>98</v>
-      </c>
+      <c r="R40" s="20"/>
+      <c r="S40" s="24"/>
       <c r="T40" s="20"/>
       <c r="U40" s="20"/>
       <c r="V40" s="20"/>
@@ -3662,11 +3756,10 @@
       <c r="AG40" s="20"/>
       <c r="AH40" s="20"/>
       <c r="AI40" s="20"/>
-      <c r="AJ40" s="24"/>
+      <c r="AJ40" s="20"/>
       <c r="AK40" s="20"/>
       <c r="AL40" s="20"/>
-      <c r="AM40" s="24"/>
-      <c r="AN40" s="24"/>
+      <c r="AN40" s="20"/>
       <c r="AO40" s="21"/>
       <c r="AP40" s="21"/>
       <c r="AQ40" s="21"/>
@@ -3679,17 +3772,19 @@
       <c r="AX40" s="21"/>
       <c r="AY40" s="21"/>
       <c r="AZ40" s="21"/>
-    </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA40" s="21"/>
+      <c r="BB40" s="21"/>
+    </row>
+    <row r="41" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A41" s="29"/>
       <c r="B41" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C41" s="20"/>
       <c r="D41" s="24"/>
-      <c r="E41" s="20"/>
+      <c r="E41" s="34"/>
       <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
@@ -3698,16 +3793,14 @@
       <c r="M41" s="24"/>
       <c r="N41" s="24"/>
       <c r="O41" s="20"/>
-      <c r="P41" s="24"/>
-      <c r="Q41" s="24"/>
-      <c r="R41" s="24"/>
-      <c r="S41" s="24" t="s">
-        <v>98</v>
-      </c>
+      <c r="P41" s="20"/>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="20"/>
       <c r="T41" s="20"/>
       <c r="U41" s="20"/>
       <c r="V41" s="20"/>
-      <c r="W41" s="24"/>
+      <c r="W41" s="20"/>
       <c r="X41" s="24"/>
       <c r="Y41" s="24"/>
       <c r="Z41" s="20"/>
@@ -3720,12 +3813,14 @@
       <c r="AG41" s="20"/>
       <c r="AH41" s="20"/>
       <c r="AI41" s="20"/>
-      <c r="AJ41" s="24"/>
-      <c r="AK41" s="20"/>
+      <c r="AJ41" s="20"/>
+      <c r="AK41" s="24"/>
       <c r="AL41" s="20"/>
-      <c r="AM41" s="24"/>
-      <c r="AN41" s="24"/>
-      <c r="AO41" s="24"/>
+      <c r="AM41" s="20"/>
+      <c r="AN41" s="20"/>
+      <c r="AO41" s="24" t="s">
+        <v>104</v>
+      </c>
       <c r="AP41" s="21"/>
       <c r="AQ41" s="21"/>
       <c r="AR41" s="21"/>
@@ -3737,11 +3832,13 @@
       <c r="AX41" s="21"/>
       <c r="AY41" s="21"/>
       <c r="AZ41" s="21"/>
-    </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA41" s="21"/>
+      <c r="BB41" s="21"/>
+    </row>
+    <row r="42" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A42" s="29"/>
       <c r="B42" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42" s="20"/>
       <c r="D42" s="24"/>
@@ -3756,8 +3853,8 @@
       <c r="M42" s="24"/>
       <c r="N42" s="24"/>
       <c r="O42" s="20"/>
-      <c r="P42" s="20"/>
-      <c r="Q42" s="20"/>
+      <c r="P42" s="24"/>
+      <c r="Q42" s="24"/>
       <c r="R42" s="24"/>
       <c r="S42" s="24" t="s">
         <v>98</v>
@@ -3766,8 +3863,8 @@
       <c r="U42" s="20"/>
       <c r="V42" s="20"/>
       <c r="W42" s="24"/>
-      <c r="X42" s="20"/>
-      <c r="Y42" s="20"/>
+      <c r="X42" s="24"/>
+      <c r="Y42" s="24"/>
       <c r="Z42" s="20"/>
       <c r="AA42" s="20"/>
       <c r="AB42" s="20"/>
@@ -3779,10 +3876,10 @@
       <c r="AH42" s="20"/>
       <c r="AI42" s="20"/>
       <c r="AJ42" s="20"/>
-      <c r="AK42" s="20"/>
+      <c r="AK42" s="24"/>
       <c r="AL42" s="20"/>
       <c r="AM42" s="20"/>
-      <c r="AN42" s="24"/>
+      <c r="AN42" s="20"/>
       <c r="AO42" s="24"/>
       <c r="AP42" s="24"/>
       <c r="AQ42" s="21"/>
@@ -3795,37 +3892,37 @@
       <c r="AX42" s="21"/>
       <c r="AY42" s="21"/>
       <c r="AZ42" s="21"/>
-    </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA42" s="21"/>
+      <c r="BB42" s="21"/>
+    </row>
+    <row r="43" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A43" s="29"/>
       <c r="B43" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C43" s="20"/>
       <c r="D43" s="24"/>
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
-      <c r="G43" s="24"/>
+      <c r="G43" s="20"/>
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
-      <c r="K43" s="24"/>
+      <c r="K43" s="20"/>
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
       <c r="N43" s="24"/>
       <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="24"/>
+      <c r="R43" s="24"/>
       <c r="S43" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="T43" s="24" t="s">
-        <v>107</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="T43" s="20"/>
       <c r="U43" s="20"/>
       <c r="V43" s="20"/>
-      <c r="W43" s="20"/>
+      <c r="W43" s="24"/>
       <c r="X43" s="24"/>
       <c r="Y43" s="24"/>
       <c r="Z43" s="20"/>
@@ -3838,13 +3935,13 @@
       <c r="AG43" s="20"/>
       <c r="AH43" s="20"/>
       <c r="AI43" s="20"/>
-      <c r="AJ43" s="24"/>
-      <c r="AK43" s="20"/>
+      <c r="AJ43" s="20"/>
+      <c r="AK43" s="24"/>
       <c r="AL43" s="20"/>
       <c r="AM43" s="20"/>
       <c r="AN43" s="20"/>
-      <c r="AO43" s="20"/>
-      <c r="AP43" s="20"/>
+      <c r="AO43" s="24"/>
+      <c r="AP43" s="24"/>
       <c r="AQ43" s="24"/>
       <c r="AR43" s="21"/>
       <c r="AS43" s="21"/>
@@ -3855,28 +3952,22 @@
       <c r="AX43" s="21"/>
       <c r="AY43" s="21"/>
       <c r="AZ43" s="21"/>
-    </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A44" s="35"/>
+      <c r="BA43" s="21"/>
+      <c r="BB43" s="21"/>
+    </row>
+    <row r="44" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A44" s="29"/>
       <c r="B44" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44" s="20"/>
       <c r="D44" s="24"/>
       <c r="E44" s="20"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H44" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="I44" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="J44" s="24" t="s">
-        <v>82</v>
-      </c>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
       <c r="K44" s="20"/>
       <c r="L44" s="24"/>
       <c r="M44" s="24"/>
@@ -3884,12 +3975,14 @@
       <c r="O44" s="20"/>
       <c r="P44" s="20"/>
       <c r="Q44" s="20"/>
-      <c r="R44" s="20"/>
-      <c r="S44" s="20"/>
-      <c r="T44" s="24"/>
+      <c r="R44" s="24"/>
+      <c r="S44" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="T44" s="20"/>
       <c r="U44" s="20"/>
-      <c r="V44" s="24"/>
-      <c r="W44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="24"/>
       <c r="X44" s="20"/>
       <c r="Y44" s="20"/>
       <c r="Z44" s="20"/>
@@ -3908,11 +4001,9 @@
       <c r="AM44" s="20"/>
       <c r="AN44" s="20"/>
       <c r="AO44" s="20"/>
-      <c r="AP44" s="20"/>
-      <c r="AQ44" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR44" s="20"/>
+      <c r="AP44" s="24"/>
+      <c r="AQ44" s="24"/>
+      <c r="AR44" s="24"/>
       <c r="AS44" s="21"/>
       <c r="AT44" s="21"/>
       <c r="AU44" s="21"/>
@@ -3921,38 +4012,42 @@
       <c r="AX44" s="21"/>
       <c r="AY44" s="21"/>
       <c r="AZ44" s="21"/>
-    </row>
-    <row r="45" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A45" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" s="37" t="s">
-        <v>49</v>
+      <c r="BA44" s="21"/>
+      <c r="BB44" s="21"/>
+    </row>
+    <row r="45" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A45" s="29"/>
+      <c r="B45" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="25"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
+      <c r="G45" s="24"/>
       <c r="H45" s="20"/>
-      <c r="I45" s="24"/>
+      <c r="I45" s="20"/>
       <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
+      <c r="K45" s="24"/>
       <c r="L45" s="24"/>
-      <c r="M45" s="20"/>
+      <c r="M45" s="24"/>
       <c r="N45" s="24"/>
       <c r="O45" s="20"/>
       <c r="P45" s="20"/>
       <c r="Q45" s="20"/>
       <c r="R45" s="20"/>
-      <c r="S45" s="20"/>
-      <c r="T45" s="20"/>
+      <c r="S45" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="T45" s="24" t="s">
+        <v>107</v>
+      </c>
       <c r="U45" s="20"/>
       <c r="V45" s="20"/>
       <c r="W45" s="20"/>
-      <c r="X45" s="20"/>
-      <c r="Y45" s="20"/>
-      <c r="Z45" s="20"/>
+      <c r="X45" s="24"/>
+      <c r="Y45" s="24"/>
+      <c r="Z45" s="24"/>
       <c r="AA45" s="20"/>
       <c r="AB45" s="20"/>
       <c r="AC45" s="20"/>
@@ -3963,15 +4058,15 @@
       <c r="AH45" s="20"/>
       <c r="AI45" s="20"/>
       <c r="AJ45" s="20"/>
-      <c r="AK45" s="20"/>
+      <c r="AK45" s="24"/>
       <c r="AL45" s="20"/>
-      <c r="AM45" s="20"/>
+      <c r="AM45" s="24"/>
       <c r="AN45" s="20"/>
       <c r="AO45" s="20"/>
       <c r="AP45" s="20"/>
       <c r="AQ45" s="20"/>
       <c r="AR45" s="20"/>
-      <c r="AS45" s="20"/>
+      <c r="AS45" s="24"/>
       <c r="AT45" s="21"/>
       <c r="AU45" s="21"/>
       <c r="AV45" s="21"/>
@@ -3979,38 +4074,46 @@
       <c r="AX45" s="21"/>
       <c r="AY45" s="21"/>
       <c r="AZ45" s="21"/>
-    </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A46" s="36"/>
-      <c r="B46" s="37" t="s">
-        <v>50</v>
+      <c r="BA45" s="21"/>
+      <c r="BB45" s="21"/>
+    </row>
+    <row r="46" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A46" s="35"/>
+      <c r="B46" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
+      <c r="D46" s="24"/>
       <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="H46" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I46" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="J46" s="24" t="s">
+        <v>82</v>
+      </c>
       <c r="K46" s="20"/>
       <c r="L46" s="24"/>
-      <c r="M46" s="20"/>
+      <c r="M46" s="24"/>
       <c r="N46" s="24"/>
       <c r="O46" s="20"/>
       <c r="P46" s="20"/>
       <c r="Q46" s="20"/>
       <c r="R46" s="20"/>
       <c r="S46" s="20"/>
-      <c r="T46" s="20"/>
+      <c r="T46" s="24"/>
       <c r="U46" s="20"/>
-      <c r="V46" s="20"/>
+      <c r="V46" s="24"/>
       <c r="W46" s="20"/>
       <c r="X46" s="20"/>
       <c r="Y46" s="20"/>
-      <c r="Z46" s="24" t="s">
-        <v>89</v>
-      </c>
+      <c r="Z46" s="20"/>
       <c r="AA46" s="20"/>
       <c r="AB46" s="20"/>
       <c r="AC46" s="20"/>
@@ -4029,7 +4132,9 @@
       <c r="AP46" s="20"/>
       <c r="AQ46" s="20"/>
       <c r="AR46" s="20"/>
-      <c r="AS46" s="20"/>
+      <c r="AS46" s="49" t="s">
+        <v>72</v>
+      </c>
       <c r="AT46" s="20"/>
       <c r="AU46" s="21"/>
       <c r="AV46" s="21"/>
@@ -4037,19 +4142,23 @@
       <c r="AX46" s="21"/>
       <c r="AY46" s="21"/>
       <c r="AZ46" s="21"/>
-    </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A47" s="36"/>
+      <c r="BA46" s="21"/>
+      <c r="BB46" s="21"/>
+    </row>
+    <row r="47" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A47" s="36" t="s">
+        <v>53</v>
+      </c>
       <c r="B47" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C47" s="20"/>
       <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
+      <c r="E47" s="25"/>
       <c r="F47" s="20"/>
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
+      <c r="I47" s="24"/>
       <c r="J47" s="20"/>
       <c r="K47" s="20"/>
       <c r="L47" s="24"/>
@@ -4066,9 +4175,7 @@
       <c r="W47" s="20"/>
       <c r="X47" s="20"/>
       <c r="Y47" s="20"/>
-      <c r="Z47" s="24" t="s">
-        <v>89</v>
-      </c>
+      <c r="Z47" s="20"/>
       <c r="AA47" s="20"/>
       <c r="AB47" s="20"/>
       <c r="AC47" s="20"/>
@@ -4095,21 +4202,21 @@
       <c r="AX47" s="21"/>
       <c r="AY47" s="21"/>
       <c r="AZ47" s="21"/>
-    </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA47" s="21"/>
+      <c r="BB47" s="21"/>
+    </row>
+    <row r="48" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A48" s="36"/>
       <c r="B48" s="37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" s="20"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24" t="s">
-        <v>79</v>
-      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
       <c r="H48" s="20"/>
-      <c r="I48" s="24"/>
+      <c r="I48" s="20"/>
       <c r="J48" s="20"/>
       <c r="K48" s="20"/>
       <c r="L48" s="24"/>
@@ -4124,10 +4231,12 @@
       <c r="U48" s="20"/>
       <c r="V48" s="20"/>
       <c r="W48" s="20"/>
-      <c r="X48" s="28"/>
-      <c r="Y48" s="28"/>
+      <c r="X48" s="20"/>
+      <c r="Y48" s="20"/>
       <c r="Z48" s="20"/>
-      <c r="AA48" s="20"/>
+      <c r="AA48" s="24" t="s">
+        <v>89</v>
+      </c>
       <c r="AB48" s="20"/>
       <c r="AC48" s="20"/>
       <c r="AD48" s="20"/>
@@ -4139,13 +4248,9 @@
       <c r="AJ48" s="20"/>
       <c r="AK48" s="20"/>
       <c r="AL48" s="20"/>
-      <c r="AM48" s="24"/>
-      <c r="AN48" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="AO48" s="25" t="s">
-        <v>78</v>
-      </c>
+      <c r="AM48" s="20"/>
+      <c r="AN48" s="20"/>
+      <c r="AO48" s="20"/>
       <c r="AP48" s="20"/>
       <c r="AQ48" s="20"/>
       <c r="AR48" s="20"/>
@@ -4157,55 +4262,41 @@
       <c r="AX48" s="21"/>
       <c r="AY48" s="21"/>
       <c r="AZ48" s="21"/>
-    </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A49" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49" s="39" t="s">
-        <v>55</v>
+      <c r="BA48" s="21"/>
+      <c r="BB48" s="21"/>
+    </row>
+    <row r="49" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A49" s="36"/>
+      <c r="B49" s="37" t="s">
+        <v>51</v>
       </c>
       <c r="C49" s="20"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
-      <c r="K49" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="L49" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="M49" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="N49" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="O49" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="P49" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q49" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="R49" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="S49" s="24"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="20"/>
+      <c r="P49" s="20"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="20"/>
+      <c r="S49" s="20"/>
       <c r="T49" s="20"/>
       <c r="U49" s="20"/>
       <c r="V49" s="20"/>
-      <c r="W49" s="24"/>
+      <c r="W49" s="20"/>
       <c r="X49" s="20"/>
       <c r="Y49" s="20"/>
       <c r="Z49" s="20"/>
-      <c r="AA49" s="20"/>
+      <c r="AA49" s="24" t="s">
+        <v>89</v>
+      </c>
       <c r="AB49" s="20"/>
       <c r="AC49" s="20"/>
       <c r="AD49" s="20"/>
@@ -4224,33 +4315,35 @@
       <c r="AQ49" s="20"/>
       <c r="AR49" s="20"/>
       <c r="AS49" s="20"/>
-      <c r="AT49" s="24"/>
-      <c r="AU49" s="24"/>
-      <c r="AV49" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="AW49" s="24"/>
+      <c r="AT49" s="20"/>
+      <c r="AU49" s="20"/>
+      <c r="AV49" s="20"/>
+      <c r="AW49" s="20"/>
       <c r="AX49" s="21"/>
       <c r="AY49" s="21"/>
       <c r="AZ49" s="21"/>
-    </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A50" s="38"/>
-      <c r="B50" s="39" t="s">
-        <v>56</v>
+      <c r="BA49" s="21"/>
+      <c r="BB49" s="21"/>
+    </row>
+    <row r="50" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A50" s="36"/>
+      <c r="B50" s="37" t="s">
+        <v>52</v>
       </c>
       <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24" t="s">
+        <v>79</v>
+      </c>
       <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
+      <c r="I50" s="24"/>
       <c r="J50" s="20"/>
       <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
+      <c r="L50" s="24"/>
       <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
+      <c r="N50" s="24"/>
       <c r="O50" s="20"/>
       <c r="P50" s="20"/>
       <c r="Q50" s="20"/>
@@ -4260,8 +4353,8 @@
       <c r="U50" s="20"/>
       <c r="V50" s="20"/>
       <c r="W50" s="20"/>
-      <c r="X50" s="20"/>
-      <c r="Y50" s="20"/>
+      <c r="X50" s="28"/>
+      <c r="Y50" s="28"/>
       <c r="Z50" s="20"/>
       <c r="AA50" s="20"/>
       <c r="AB50" s="20"/>
@@ -4277,117 +4370,127 @@
       <c r="AL50" s="20"/>
       <c r="AM50" s="20"/>
       <c r="AN50" s="20"/>
-      <c r="AO50" s="20"/>
-      <c r="AP50" s="20"/>
-      <c r="AQ50" s="20"/>
+      <c r="AO50" s="24"/>
+      <c r="AP50" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ50" s="25" t="s">
+        <v>78</v>
+      </c>
       <c r="AR50" s="20"/>
       <c r="AS50" s="20"/>
       <c r="AT50" s="20"/>
       <c r="AU50" s="20"/>
-      <c r="AV50" s="24"/>
+      <c r="AV50" s="20"/>
       <c r="AW50" s="20"/>
       <c r="AX50" s="20"/>
       <c r="AY50" s="21"/>
       <c r="AZ50" s="21"/>
-    </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A51" s="38"/>
+      <c r="BA50" s="21"/>
+      <c r="BB50" s="21"/>
+    </row>
+    <row r="51" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A51" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="B51" s="39" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="24" t="s">
-        <v>71</v>
-      </c>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
       <c r="F51" s="20"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
       <c r="J51" s="20"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="20"/>
-      <c r="Q51" s="20"/>
-      <c r="R51" s="20"/>
-      <c r="S51" s="24" t="s">
-        <v>98</v>
-      </c>
+      <c r="K51" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="L51" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="M51" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="N51" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="O51" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="P51" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q51" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="R51" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="S51" s="24"/>
       <c r="T51" s="20"/>
       <c r="U51" s="20"/>
-      <c r="V51" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="W51" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="X51" s="24"/>
-      <c r="Y51" s="24"/>
+      <c r="V51" s="20"/>
+      <c r="W51" s="24"/>
+      <c r="X51" s="20"/>
+      <c r="Y51" s="20"/>
       <c r="Z51" s="20"/>
       <c r="AA51" s="20"/>
       <c r="AB51" s="20"/>
-      <c r="AC51" s="24" t="s">
-        <v>110</v>
-      </c>
+      <c r="AC51" s="20"/>
       <c r="AD51" s="20"/>
       <c r="AE51" s="20"/>
       <c r="AF51" s="20"/>
-      <c r="AG51" s="24"/>
-      <c r="AH51" s="24"/>
-      <c r="AI51" s="24"/>
+      <c r="AG51" s="20"/>
+      <c r="AH51" s="20"/>
+      <c r="AI51" s="20"/>
       <c r="AJ51" s="20"/>
       <c r="AK51" s="20"/>
-      <c r="AL51" s="24"/>
-      <c r="AM51" s="24"/>
-      <c r="AN51" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="AO51" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP51" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="AQ51" s="24"/>
+      <c r="AL51" s="20"/>
+      <c r="AM51" s="20"/>
+      <c r="AN51" s="20"/>
+      <c r="AO51" s="20"/>
+      <c r="AP51" s="20"/>
+      <c r="AQ51" s="20"/>
       <c r="AR51" s="20"/>
-      <c r="AS51" s="24"/>
+      <c r="AS51" s="20"/>
       <c r="AT51" s="20"/>
       <c r="AU51" s="20"/>
       <c r="AV51" s="24"/>
-      <c r="AW51" s="20"/>
-      <c r="AX51" s="24"/>
-      <c r="AY51" s="20"/>
+      <c r="AW51" s="24"/>
+      <c r="AX51" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY51" s="24"/>
       <c r="AZ51" s="21"/>
-    </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="BA51" s="21"/>
+      <c r="BB51" s="21"/>
+    </row>
+    <row r="52" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A52" s="38"/>
       <c r="B52" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="C52" s="40"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="41"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="41"/>
-      <c r="H52" s="41"/>
-      <c r="I52" s="41"/>
-      <c r="J52" s="41"/>
-      <c r="K52" s="41"/>
-      <c r="L52" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="M52" s="41"/>
-      <c r="N52" s="41"/>
-      <c r="O52" s="41"/>
-      <c r="P52" s="41"/>
-      <c r="Q52" s="41"/>
-      <c r="R52" s="41"/>
-      <c r="S52" s="41"/>
-      <c r="T52" s="41"/>
-      <c r="U52" s="41"/>
+        <v>56</v>
+      </c>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="20"/>
+      <c r="R52" s="20"/>
+      <c r="S52" s="20"/>
+      <c r="T52" s="20"/>
+      <c r="U52" s="20"/>
       <c r="V52" s="20"/>
       <c r="W52" s="20"/>
       <c r="X52" s="20"/>
@@ -4414,39 +4517,123 @@
       <c r="AS52" s="20"/>
       <c r="AT52" s="20"/>
       <c r="AU52" s="20"/>
-      <c r="AV52" s="24"/>
+      <c r="AV52" s="20"/>
       <c r="AW52" s="20"/>
       <c r="AX52" s="24"/>
-      <c r="AY52" s="24"/>
-      <c r="AZ52" s="24"/>
-    </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.35">
+      <c r="AY52" s="20"/>
+      <c r="AZ52" s="20"/>
+      <c r="BA52" s="21"/>
+      <c r="BB52" s="21"/>
+    </row>
+    <row r="53" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A53" s="38"/>
+      <c r="B53" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="20"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="24"/>
+      <c r="L53" s="20"/>
+      <c r="M53" s="20"/>
+      <c r="N53" s="20"/>
+      <c r="O53" s="20"/>
+      <c r="P53" s="20"/>
+      <c r="Q53" s="20"/>
+      <c r="R53" s="20"/>
+      <c r="S53" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="T53" s="20"/>
+      <c r="U53" s="20"/>
+      <c r="V53" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="W53" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="X53" s="24"/>
+      <c r="Y53" s="24"/>
+      <c r="Z53" s="24"/>
+      <c r="AA53" s="20"/>
+      <c r="AB53" s="20"/>
+      <c r="AC53" s="20"/>
+      <c r="AD53" s="24" t="s">
+        <v>110</v>
+      </c>
       <c r="AE53" s="20"/>
       <c r="AF53" s="20"/>
       <c r="AG53" s="20"/>
-      <c r="AH53" s="20"/>
-      <c r="AI53" s="20"/>
-      <c r="AJ53" s="20"/>
+      <c r="AH53" s="24"/>
+      <c r="AI53" s="24"/>
+      <c r="AJ53" s="24"/>
       <c r="AK53" s="20"/>
       <c r="AL53" s="20"/>
       <c r="AM53" s="20"/>
       <c r="AN53" s="20"/>
-      <c r="AO53" s="20"/>
-      <c r="AP53" s="20"/>
-      <c r="AQ53" s="20"/>
-      <c r="AR53" s="20"/>
-      <c r="AS53" s="20"/>
+      <c r="AO53" s="24"/>
+      <c r="AP53" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="AQ53" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="AR53" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="AS53" s="24"/>
       <c r="AT53" s="20"/>
-      <c r="AU53" s="20"/>
+      <c r="AU53" s="24"/>
       <c r="AV53" s="20"/>
       <c r="AW53" s="20"/>
-      <c r="AX53" s="20"/>
+      <c r="AX53" s="24"/>
       <c r="AY53" s="20"/>
-    </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.35">
-      <c r="A54" s="22" t="s">
-        <v>83</v>
-      </c>
+      <c r="AZ53" s="24"/>
+      <c r="BA53" s="20"/>
+      <c r="BB53" s="21"/>
+    </row>
+    <row r="54" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A54" s="38"/>
+      <c r="B54" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="40"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
+      <c r="G54" s="41"/>
+      <c r="H54" s="41"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="M54" s="41"/>
+      <c r="N54" s="41"/>
+      <c r="O54" s="41"/>
+      <c r="P54" s="41"/>
+      <c r="Q54" s="41"/>
+      <c r="R54" s="41"/>
+      <c r="S54" s="41"/>
+      <c r="T54" s="41"/>
+      <c r="U54" s="41"/>
+      <c r="V54" s="20"/>
+      <c r="W54" s="20"/>
+      <c r="X54" s="20"/>
+      <c r="Y54" s="20"/>
+      <c r="Z54" s="20"/>
+      <c r="AA54" s="20"/>
+      <c r="AB54" s="20"/>
+      <c r="AC54" s="20"/>
+      <c r="AD54" s="20"/>
       <c r="AE54" s="20"/>
       <c r="AF54" s="20"/>
       <c r="AG54" s="20"/>
@@ -4466,24 +4653,54 @@
       <c r="AU54" s="20"/>
       <c r="AV54" s="20"/>
       <c r="AW54" s="20"/>
-      <c r="AX54" s="20"/>
+      <c r="AX54" s="24"/>
       <c r="AY54" s="20"/>
-    </row>
-    <row r="55" spans="1:52" s="48" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="46" t="s">
+      <c r="AZ54" s="24"/>
+      <c r="BA54" s="24"/>
+      <c r="BB54" s="24"/>
+    </row>
+    <row r="55" spans="1:54" x14ac:dyDescent="0.35">
+      <c r="A55" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE55" s="20"/>
+      <c r="AF55" s="20"/>
+      <c r="AG55" s="20"/>
+      <c r="AH55" s="20"/>
+      <c r="AI55" s="20"/>
+      <c r="AJ55" s="20"/>
+      <c r="AK55" s="20"/>
+      <c r="AL55" s="20"/>
+      <c r="AM55" s="20"/>
+      <c r="AN55" s="20"/>
+      <c r="AO55" s="20"/>
+      <c r="AP55" s="20"/>
+      <c r="AQ55" s="20"/>
+      <c r="AR55" s="20"/>
+      <c r="AS55" s="20"/>
+      <c r="AT55" s="20"/>
+      <c r="AU55" s="20"/>
+      <c r="AV55" s="20"/>
+      <c r="AW55" s="20"/>
+      <c r="AX55" s="20"/>
+      <c r="AY55" s="20"/>
+      <c r="AZ55" s="20"/>
+    </row>
+    <row r="56" spans="1:54" s="48" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B55" s="47" t="s">
+      <c r="B56" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="C55" s="46" t="s">
+      <c r="C56" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="D55" s="46" t="s">
+      <c r="D56" s="46" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:54" x14ac:dyDescent="0.35">
       <c r="G59" s="43"/>
     </row>
   </sheetData>

</xml_diff>